<commit_message>
Implemented Bloch sphere plots for the results of the error correction and the results calculated from experimental data.  Also corrected an issue with writing to the excel file where it would just append a new sheet every time it ran
</commit_message>
<xml_diff>
--- a/11-19-19.xlsx
+++ b/11-19-19.xlsx
@@ -2,8 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="1" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="15840" windowWidth="29040" xWindow="-120" yWindow="-120"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
     <sheet name="measured" sheetId="1" state="visible" r:id="rId1"/>
@@ -11,7 +12,7 @@
     <sheet name="Adjusted" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="162913" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -64,9 +65,9 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -81,44 +82,44 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -145,15 +146,14 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -180,7 +180,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -192,142 +191,166 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="35000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="80000">
               <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="40000">
               <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
@@ -340,33 +363,33 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:A1048576"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>theta</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>I1</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>I2</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>I3</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>I4</t>
         </is>
@@ -696,7 +719,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
@@ -708,34 +731,34 @@
   </sheetPr>
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>theta</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Jxx</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Jyy</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>beta</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>gamma</t>
         </is>
@@ -1065,7 +1088,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
@@ -1116,611 +1139,383 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>0j</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>(0.03299004658694232+0j)</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>(0.9670099534130576+0j)</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>(0.1399727590060066+0j)</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>(0.11094742068968524+0j)</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>(1.0000000000166276+0j)</t>
-        </is>
+      <c r="A2" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0.03299004658694232</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.9670099534130576</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.1399727590060066</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.1109474206896852</v>
+      </c>
+      <c r="F2" t="n">
+        <v>1.000000000016628</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>(5+0j)</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>(0.06513311755307133+0j)</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>(0.9348668824469286+0j)</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>(0.1763817406725079+0j)</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>(0.17256962686565977+0j)</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>(1.0000000000166556+0j)</t>
-        </is>
+      <c r="A3" t="n">
+        <v>5</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0.06513311755307133</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.9348668824469286</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.1763817406725079</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.1725696268656598</v>
+      </c>
+      <c r="F3" t="n">
+        <v>1.000000000016656</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>(10+0j)</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>(0.1300531215395943+0j)</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>(0.8699468784604056+0j)</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>(0.2316260323103869+0j)</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>(0.24390303048826656+0j)</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>(1.0000000000156217+0j)</t>
-        </is>
+      <c r="A4" t="n">
+        <v>10</v>
+      </c>
+      <c r="B4" t="n">
+        <v>0.1300531215395943</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.8699468784604056</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.2316260323103869</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.2439030304882666</v>
+      </c>
+      <c r="F4" t="n">
+        <v>1.000000000015622</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>(15+0j)</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>(0.24705718081747374+0j)</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>(0.7529428191825263+0j)</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>(0.28988697646456196+0j)</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>(0.31935164177967745+0j)</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>(1.0000000000142901+0j)</t>
-        </is>
+      <c r="A5" t="n">
+        <v>15</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0.2470571808174737</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.7529428191825263</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.289886976464562</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.3193516417796775</v>
+      </c>
+      <c r="F5" t="n">
+        <v>1.00000000001429</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>(20+0j)</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>(0.4396832533266938+0j)</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>(0.5603167466733062+0j)</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>(0.3311389392364511+0j)</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>(0.3697416571050494+0j)</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>(1.0000000000133635+0j)</t>
-        </is>
+      <c r="A6" t="n">
+        <v>20</v>
+      </c>
+      <c r="B6" t="n">
+        <v>0.4396832533266938</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.5603167466733062</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.3311389392364511</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.3697416571050494</v>
+      </c>
+      <c r="F6" t="n">
+        <v>1.000000000013364</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>(25+0j)</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>(0.655003049564529+0j)</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>(0.34499695043547096+0j)</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>(0.32174875439909817+0j)</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>(0.3499311270449942+0j)</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>(1.0000000000133098+0j)</t>
-        </is>
+      <c r="A7" t="n">
+        <v>25</v>
+      </c>
+      <c r="B7" t="n">
+        <v>0.655003049564529</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.344996950435471</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.3217487543990982</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.3499311270449942</v>
+      </c>
+      <c r="F7" t="n">
+        <v>1.00000000001331</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>(30+0j)</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>(0.8140844524977702+0j)</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>(0.18591554750222983+0j)</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>(0.27300387013465144+0j)</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>(0.2771639291065034+0j)</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>(1.000000000014153+0j)</t>
-        </is>
+      <c r="A8" t="n">
+        <v>30</v>
+      </c>
+      <c r="B8" t="n">
+        <v>0.8140844524977702</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.1859155475022298</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.2730038701346514</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.2771639291065034</v>
+      </c>
+      <c r="F8" t="n">
+        <v>1.000000000014153</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>(35+0j)</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>(0.9064336979649437+0j)</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>(0.09356630203505639+0j)</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>(0.2157239057257777+0j)</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>(0.19563958102754994+0j)</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>(1.000000000015357+0j)</t>
-        </is>
+      <c r="A9" t="n">
+        <v>35</v>
+      </c>
+      <c r="B9" t="n">
+        <v>0.9064336979649437</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.09356630203505639</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.2157239057257777</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.1956395810275499</v>
+      </c>
+      <c r="F9" t="n">
+        <v>1.000000000015357</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>(40+0j)</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>(0.9513752907290096+0j)</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>(0.04862470927099044+0j)</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>(0.17464126496135537+0j)</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>(0.12554192725963967+0j)</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>(1.0000000000161298+0j)</t>
-        </is>
+      <c r="A10" t="n">
+        <v>40</v>
+      </c>
+      <c r="B10" t="n">
+        <v>0.9513752907290096</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.04862470927099044</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.1746412649613554</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.1255419272596397</v>
+      </c>
+      <c r="F10" t="n">
+        <v>1.00000000001613</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>(45+0j)</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>(0.9784116748449645+0j)</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>(0.021588325155035448+0j)</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>(0.13390999127987285+0j)</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>(0.056483480908222514+0j)</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>(1.0000000000160982+0j)</t>
-        </is>
+      <c r="A11" t="n">
+        <v>45</v>
+      </c>
+      <c r="B11" t="n">
+        <v>0.9784116748449645</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.02158832515503545</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.1339099912798729</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.05648348090822251</v>
+      </c>
+      <c r="F11" t="n">
+        <v>1.000000000016098</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>(50+0j)</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>(0.9877332822396789+0j)</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>(0.012266717760321122+0j)</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>(0.11004184893742193+0j)</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>(-0.002652712900390008+0j)</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>(1.0000000000151772+0j)</t>
-        </is>
+      <c r="A12" t="n">
+        <v>50</v>
+      </c>
+      <c r="B12" t="n">
+        <v>0.9877332822396789</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.01226671776032112</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.1100418489374219</v>
+      </c>
+      <c r="E12" t="n">
+        <v>-0.002652712900390008</v>
+      </c>
+      <c r="F12" t="n">
+        <v>1.000000000015177</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>(55+0j)</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>(0.9867319386047305+0j)</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>(0.013268061395269481+0j)</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>(0.0924970289230393+0j)</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>(-0.06735220552606468+0j)</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>(1.000000000013468+0j)</t>
-        </is>
+      <c r="A13" t="n">
+        <v>55</v>
+      </c>
+      <c r="B13" t="n">
+        <v>0.9867319386047305</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.01326806139526948</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.09249702892303931</v>
+      </c>
+      <c r="E13" t="n">
+        <v>-0.06735220552606468</v>
+      </c>
+      <c r="F13" t="n">
+        <v>1.000000000013468</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>(60+0j)</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>(0.9693638867586813+0j)</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>(0.030636113241318652+0j)</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>(0.08738814470572813+0j)</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>(-0.14852896679583308+0j)</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>(1.0000000000115266+0j)</t>
-        </is>
+      <c r="A14" t="n">
+        <v>60</v>
+      </c>
+      <c r="B14" t="n">
+        <v>0.9693638867586813</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.03063611324131865</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.08738814470572813</v>
+      </c>
+      <c r="E14" t="n">
+        <v>-0.1485289667958331</v>
+      </c>
+      <c r="F14" t="n">
+        <v>1.000000000011527</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>(65+0j)</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>(0.8638455419258018+0j)</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>(0.13615445807419818+0j)</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>(0.11810541797432786+0j)</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>(-0.3219744279725793+0j)</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>(1.0000000008048815+0j)</t>
-        </is>
+      <c r="A15" t="n">
+        <v>65</v>
+      </c>
+      <c r="B15" t="n">
+        <v>0.8638455419258018</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.1361544580741982</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.1181054179743279</v>
+      </c>
+      <c r="E15" t="n">
+        <v>-0.3219744279725793</v>
+      </c>
+      <c r="F15" t="n">
+        <v>1.000000000804881</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>(70+0j)</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>(0.2924111537384785+0j)</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>(0.7075888462615215+0j)</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>(0.16953089111357592+0j)</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>(-0.42209732073828066+0j)</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>(1.0000000006167755+0j)</t>
-        </is>
+      <c r="A16" t="n">
+        <v>70</v>
+      </c>
+      <c r="B16" t="n">
+        <v>0.2924111537384785</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0.7075888462615215</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.1695308911135759</v>
+      </c>
+      <c r="E16" t="n">
+        <v>-0.4220973207382807</v>
+      </c>
+      <c r="F16" t="n">
+        <v>1.000000000616776</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>(75+0j)</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>(0.02941860352288639+0j)</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>(0.9705813964771136+0j)</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>(0.11030600623844272+0j)</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>(-0.12800677436231325+0j)</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>(1.00000000001054+0j)</t>
-        </is>
+      <c r="A17" t="n">
+        <v>75</v>
+      </c>
+      <c r="B17" t="n">
+        <v>0.02941860352288639</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0.9705813964771136</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.1103060062384427</v>
+      </c>
+      <c r="E17" t="n">
+        <v>-0.1280067743623133</v>
+      </c>
+      <c r="F17" t="n">
+        <v>1.00000000001054</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>(80+0j)</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>(0.011242440429940936+0j)</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>(0.9887575595700591+0j)</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>(0.10516939362193808+0j)</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>(-0.007446248368329971+0j)</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>(1.0000000000128977+0j)</t>
-        </is>
+      <c r="A18" t="n">
+        <v>80</v>
+      </c>
+      <c r="B18" t="n">
+        <v>0.01124244042994094</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0.9887575595700591</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0.1051693936219381</v>
+      </c>
+      <c r="E18" t="n">
+        <v>-0.007446248368329971</v>
+      </c>
+      <c r="F18" t="n">
+        <v>1.000000000012898</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>(85+0j)</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>(0.018834504098972304+0j)</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>(0.9811654959010276+0j)</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>(0.11695118402777663+0j)</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>(0.06929780744338339+0j)</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>(1.0000000000152818+0j)</t>
-        </is>
+      <c r="A19" t="n">
+        <v>85</v>
+      </c>
+      <c r="B19" t="n">
+        <v>0.0188345040989723</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0.9811654959010276</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0.1169511840277766</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0.06929780744338339</v>
+      </c>
+      <c r="F19" t="n">
+        <v>1.000000000015282</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>(90+0j)</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>(0.03883803075486181+0j)</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>(0.9611619692451382+0j)</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>(0.13962750055684575+0j)</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>(0.13354324849500743+0j)</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>(1.00000000001681+0j)</t>
-        </is>
+      <c r="A20" t="n">
+        <v>90</v>
+      </c>
+      <c r="B20" t="n">
+        <v>0.03883803075486181</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0.9611619692451382</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0.1396275005568458</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0.1335432484950074</v>
+      </c>
+      <c r="F20" t="n">
+        <v>1.00000000001681</v>
       </c>
     </row>
   </sheetData>

</xml_diff>